<commit_message>
Master Powershell Udemy almost at the end && JavaScript for C# Developers started.
</commit_message>
<xml_diff>
--- a/Common_Language_Features.xlsx
+++ b/Common_Language_Features.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC10090-AD0E-4898-8724-2EF52A8D8F59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4C1C99-D69D-4EEA-B1CF-15AA0C41B32C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{08F49B87-7F4B-4922-8412-B2D12D0AD46C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These are useful when you want to refer to a specific value all the time otherwise it would require to iterate through all the items in the list
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{0FBA9DCC-6C44-4A8B-B494-06901EE4BB70}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Functions allow us to reuse code.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
   <si>
     <t>Features ▼</t>
   </si>
@@ -944,13 +1003,190 @@
   </si>
   <si>
     <t>Powershell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loops </t>
+  </si>
+  <si>
+    <t>Loops - FOREACH</t>
+  </si>
+  <si>
+    <t>1..10 | foreach {$_*2}</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>$serverComputers = @("Server1", "Server2", "Server3")</t>
+  </si>
+  <si>
+    <t>Dictionary/HashMap/HashTables
+-Collection of key value pairs</t>
+  </si>
+  <si>
+    <t>$empNumbers = @("Ranjit" = 2289, "Venkat" = 1234)</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Calling/Executing Functions</t>
+  </si>
+  <si>
+    <t>function Add-Numbers
+{
+     param([int]$num1, [int]$num2)
+$num1 + $num2
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a) Add-Numbers 123 456 
+b) Add-Numbers -num1 123 -num2 456
+c) $result = Add-Numbers -num1 123 -num2 456
+$result </t>
+  </si>
+  <si>
+    <t>RUNTIME Environments</t>
+  </si>
+  <si>
+    <t>runs inside the CLR</t>
+  </si>
+  <si>
+    <t>Have variety of engines on which your code can run.   These typically depends on the browser.  Ex:  V8 in chrome, Chakra in IE</t>
+  </si>
+  <si>
+    <t>SERVICES of Runtime Environments</t>
+  </si>
+  <si>
+    <t>Memory Mgmt
+JUST In Time Compilation
+Common Type System etc.</t>
+  </si>
+  <si>
+    <t>Memory Mgmt
+JUST In Time Compilation (most part)
+Type System (simplified) etc.</t>
+  </si>
+  <si>
+    <t>Typing</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Static (compiled into known types) (most part of c# its static though dynamic keyword is supported)</t>
+  </si>
+  <si>
+    <t>Dynamic  (Shapes are important but identity is less important) (you can add-on or tear off parts of the structure easily than in other languages)</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Classical Inheritance</t>
+  </si>
+  <si>
+    <t>Prototypical Inheritance
+- but method of doing this is fairly different</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Constructors</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>Namespace/Dlls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dispersed class support for Functions.
+They use Functions to micic functions that are like classes, constructors, methods etc. </t>
+  </si>
+  <si>
+    <t>var keyword</t>
+  </si>
+  <si>
+    <t>Compiler infers the type of the variable</t>
+  </si>
+  <si>
+    <t>variable declaration</t>
+  </si>
+  <si>
+    <t>Strongly-Typed
+- Types are defined by names and static structures
+- Compiler does the checks and infers the type for you
+- INHERITANCE and IMPLEMENTATIONS are part of type identity (When a class implements an interface then we are sure that the class have this functionality, methods etc.)</t>
+  </si>
+  <si>
+    <t>Loosely-Typed
+- Types are defined by structure and not by identity
+- Runtime checks but NOT compile time
+- Type is less important, but shape is important (i.e. if characteristics matches any structure is fine)</t>
+  </si>
+  <si>
+    <t>Dynamic Typing</t>
+  </si>
+  <si>
+    <t>Using dynamic keyword you can do some dynamic functionality</t>
+  </si>
+  <si>
+    <t>You can add on to OR remove parts(properties OR methods) of the implementation as needed</t>
+  </si>
+  <si>
+    <t>Global Scope</t>
+  </si>
+  <si>
+    <t>All code takes place inside of the class and any member  can be part of this class and will be inside the scope of this class</t>
+  </si>
+  <si>
+    <t>Objects (variable, function etc.) at root are 'GLOBAL'
+-  You can think of this as command line parser.</t>
+  </si>
+  <si>
+    <t>Closures</t>
+  </si>
+  <si>
+    <t>Supported</t>
+  </si>
+  <si>
+    <t>References outside of function are accessible in function with Regardless of lifetime
+- functionality is SAME AS in other languages</t>
+  </si>
+  <si>
+    <t>Coalesce</t>
+  </si>
+  <si>
+    <t>This Coalesce values by default</t>
+  </si>
+  <si>
+    <t>Operators</t>
+  </si>
+  <si>
+    <t>Identically Equality Operators</t>
+  </si>
+  <si>
+    <t>- So for this purpose  (===, !==) have come.   These determines equality without COALESCING</t>
+  </si>
+  <si>
+    <t>Most operators identical to .NET except (==, !=)
+-  Determines equality with coalescing (if necessary to do comparision).   Example 1 == "1" //which is true in JavaScript.   So there are times where we don't want this behaviour.</t>
+  </si>
+  <si>
+    <t>Object.Equals()
+- Determines whether two objects are same without Coalescing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,6 +1283,19 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1121,7 +1370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1157,6 +1406,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1437,71 +1695,295 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="100.8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2">
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2">
+      <c r="B6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
+      <c r="B7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="72">
+      <c r="B9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.2">
+      <c r="B10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8">
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2">
+      <c r="B15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
+    <row r="18" spans="2:5">
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+    <row r="19" spans="2:5">
+      <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+    <row r="20" spans="2:5">
+      <c r="B20" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="28.8">
+      <c r="B24" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="72">
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="57.6">
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="43.2">
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Javascript Notes completed _ Base notes is ready
</commit_message>
<xml_diff>
--- a/Common_Language_Features.xlsx
+++ b/Common_Language_Features.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4C1C99-D69D-4EEA-B1CF-15AA0C41B32C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624A416B-278B-4A34-897C-28253DA005D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,10 +12,16 @@
     <sheet name="AccessModifiers" sheetId="4" r:id="rId2"/>
     <sheet name="ClassDeclaration" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,7 +33,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{08F49B87-7F4B-4922-8412-B2D12D0AD46C}">
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{08F49B87-7F4B-4922-8412-B2D12D0AD46C}">
       <text>
         <r>
           <rPr>
@@ -52,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{0FBA9DCC-6C44-4A8B-B494-06901EE4BB70}">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{0FBA9DCC-6C44-4A8B-B494-06901EE4BB70}">
       <text>
         <r>
           <rPr>
@@ -81,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
   <si>
     <t>Features ▼</t>
   </si>
@@ -1149,9 +1155,6 @@
 -  You can think of this as command line parser.</t>
   </si>
   <si>
-    <t>Closures</t>
-  </si>
-  <si>
     <t>Supported</t>
   </si>
   <si>
@@ -1180,13 +1183,165 @@
   <si>
     <t>Object.Equals()
 - Determines whether two objects are same without Coalescing</t>
+  </si>
+  <si>
+    <t>Primitive DataTypes</t>
+  </si>
+  <si>
+    <t>Type Detection</t>
+  </si>
+  <si>
+    <t>typeof operator</t>
+  </si>
+  <si>
+    <t>- Value Types = boolean, string, number
+- Reference Types = object
+- Delegate Type = function
+- Special = undefined, null</t>
+  </si>
+  <si>
+    <t>Reference Types</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All classes/objects derive from base class called </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All of the objects you are going to deal with are of type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object</t>
+    </r>
+  </si>
+  <si>
+    <t>Function Overloading</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>No OVERLOADING possible.   If you redefine the function with one more parameter then it simply overrides the first function definition</t>
+  </si>
+  <si>
+    <t>Function Return Value</t>
+  </si>
+  <si>
+    <t>Member functions don't return a value</t>
+  </si>
+  <si>
+    <t>All functions return a value.
+If not defined it's "undefined"</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Just an object 
+- Has properties and member functions</t>
+  </si>
+  <si>
+    <t>THIS keyword</t>
+  </si>
+  <si>
+    <t>Represents the instance of the class that we are working with</t>
+  </si>
+  <si>
+    <t>applies to the OWNER of the function object</t>
+  </si>
+  <si>
+    <t>THIS keyword - Changing the function execution context</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>bind() method - lets you change the owner/the context in which the function executes</t>
+  </si>
+  <si>
+    <t>Closures
+- It allows a piece of data i.e. referenced by a function to be accessed regardless of the lifetime of the function</t>
+  </si>
+  <si>
+    <t>Scoping</t>
+  </si>
+  <si>
+    <t>Exists all over the place.    Even block level scope works.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Functions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>only</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> create scope for variables.
+Block level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doesn't</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> scope a variable because of variable Hoisting</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1295,6 +1450,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1696,11 +1859,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1733,250 +1896,343 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="100.8">
-      <c r="A3">
+    <row r="3" spans="1:5" ht="57.6">
+      <c r="B3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8">
+      <c r="B4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="100.8">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
-      <c r="A4">
+    <row r="7" spans="1:5" ht="28.8">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C7" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2">
-      <c r="B5" s="3" t="s">
+    <row r="8" spans="1:5" ht="43.2">
+      <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C8" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D8" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2">
-      <c r="B6" s="3" t="s">
+    <row r="9" spans="1:5" ht="43.2">
+      <c r="B9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C9" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2">
-      <c r="B7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="72">
-      <c r="B9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2">
       <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="72">
+      <c r="B12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2">
+      <c r="B13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8">
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="28.8">
+      <c r="B14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C14" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D14" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="3" t="s">
+    <row r="15" spans="1:5">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.2">
-      <c r="B15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.8">
       <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
+        <v>105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="43.2">
       <c r="B19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8">
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="28.8">
-      <c r="B24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="72">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="28.8">
+      <c r="B22" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="72">
+      <c r="B23" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="43.2">
+      <c r="B24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="57.6">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>52</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="28.8">
+      <c r="B33" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="72">
+      <c r="B34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="57.6">
+      <c r="B35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C37" t="s">
         <v>54</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="43.2">
-      <c r="B29" s="3" t="s">
+    <row r="38" spans="2:5" ht="43.2">
+      <c r="B38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C38" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D38" s="20" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>